<commit_message>
refactor: update xmind test case to excel test case
</commit_message>
<xml_diff>
--- a/xmind2excel/template/result.xlsx
+++ b/xmind2excel/template/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7740" windowWidth="19104"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7740" windowWidth="19100" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,16 +18,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
-    <t>所属功能</t>
+    <t>功能模块</t>
   </si>
   <si>
     <t>用例标题</t>
   </si>
   <si>
-    <t>级别</t>
-  </si>
-  <si>
-    <t>前置步骤</t>
+    <t>优先级</t>
+  </si>
+  <si>
+    <t>前置条件</t>
   </si>
   <si>
     <t>执行步骤</t>
@@ -136,13 +136,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ " numFmtId="164"/>
-    <numFmt formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ " numFmtId="165"/>
-    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="166"/>
-    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="167"/>
-  </numFmts>
-  <fonts count="22">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <name val="DengXian"/>
       <charset val="134"/>
@@ -160,35 +155,6 @@
     </font>
     <font>
       <name val="DengXian"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
       <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -196,121 +162,12 @@
     </font>
     <font>
       <name val="DengXian"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -319,198 +176,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="3" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -546,318 +217,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0">
+  <cellStyleXfs count="2">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="164">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="24" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="165">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="166">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="167">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="15" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="14" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="14" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="31" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="49">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="49">
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="7" name="货币[0]" xfId="1"/>
-    <cellStyle builtinId="38" name="20% - 强调文字颜色 3" xfId="2"/>
-    <cellStyle builtinId="20" name="输入" xfId="3"/>
-    <cellStyle builtinId="4" name="货币" xfId="4"/>
-    <cellStyle builtinId="6" name="千位分隔[0]" xfId="5"/>
-    <cellStyle builtinId="39" name="40% - 强调文字颜色 3" xfId="6"/>
-    <cellStyle builtinId="27" name="差" xfId="7"/>
-    <cellStyle builtinId="3" name="千位分隔" xfId="8"/>
-    <cellStyle builtinId="40" name="60% - 强调文字颜色 3" xfId="9"/>
-    <cellStyle builtinId="8" name="超链接" xfId="10"/>
-    <cellStyle builtinId="5" name="百分比" xfId="11"/>
-    <cellStyle builtinId="9" name="已访问的超链接" xfId="12"/>
-    <cellStyle builtinId="10" name="注释" xfId="13"/>
-    <cellStyle builtinId="36" name="60% - 强调文字颜色 2" xfId="14"/>
-    <cellStyle builtinId="19" name="标题 4" xfId="15"/>
-    <cellStyle builtinId="11" name="警告文本" xfId="16"/>
-    <cellStyle builtinId="15" name="标题" xfId="17"/>
-    <cellStyle builtinId="53" name="解释性文本" xfId="18"/>
-    <cellStyle builtinId="16" name="标题 1" xfId="19"/>
-    <cellStyle builtinId="17" name="标题 2" xfId="20"/>
-    <cellStyle builtinId="32" name="60% - 强调文字颜色 1" xfId="21"/>
-    <cellStyle builtinId="18" name="标题 3" xfId="22"/>
-    <cellStyle builtinId="44" name="60% - 强调文字颜色 4" xfId="23"/>
-    <cellStyle builtinId="21" name="输出" xfId="24"/>
-    <cellStyle builtinId="22" name="计算" xfId="25"/>
-    <cellStyle builtinId="23" name="检查单元格" xfId="26"/>
-    <cellStyle builtinId="50" name="20% - 强调文字颜色 6" xfId="27"/>
-    <cellStyle builtinId="33" name="强调文字颜色 2" xfId="28"/>
-    <cellStyle builtinId="24" name="链接单元格" xfId="29"/>
-    <cellStyle builtinId="25" name="汇总" xfId="30"/>
-    <cellStyle builtinId="26" name="好" xfId="31"/>
-    <cellStyle builtinId="28" name="适中" xfId="32"/>
-    <cellStyle builtinId="46" name="20% - 强调文字颜色 5" xfId="33"/>
-    <cellStyle builtinId="29" name="强调文字颜色 1" xfId="34"/>
-    <cellStyle builtinId="30" name="20% - 强调文字颜色 1" xfId="35"/>
-    <cellStyle builtinId="31" name="40% - 强调文字颜色 1" xfId="36"/>
-    <cellStyle builtinId="34" name="20% - 强调文字颜色 2" xfId="37"/>
-    <cellStyle builtinId="35" name="40% - 强调文字颜色 2" xfId="38"/>
-    <cellStyle builtinId="37" name="强调文字颜色 3" xfId="39"/>
-    <cellStyle builtinId="41" name="强调文字颜色 4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - 强调文字颜色 4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - 强调文字颜色 4" xfId="42"/>
-    <cellStyle builtinId="45" name="强调文字颜色 5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - 强调文字颜色 5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - 强调文字颜色 5" xfId="45"/>
-    <cellStyle builtinId="49" name="强调文字颜色 6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - 强调文字颜色 6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - 强调文字颜色 6" xfId="48"/>
-    <cellStyle name="常规 2" xfId="49"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -1144,6 +525,7 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1156,21 +538,21 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="26.8333333333333"/>
-    <col customWidth="1" max="2" min="2" style="3" width="32.3333333333333"/>
-    <col customWidth="1" max="3" min="3" style="3" width="14.6666666666667"/>
+    <col customWidth="1" max="1" min="1" style="3" width="26.83203125"/>
+    <col customWidth="1" max="2" min="2" style="3" width="32.33203125"/>
+    <col customWidth="1" max="3" min="3" style="3" width="14.6640625"/>
     <col customWidth="1" max="4" min="4" style="3" width="24"/>
     <col customWidth="1" max="5" min="5" style="3" width="39"/>
     <col customWidth="1" max="6" min="6" style="3" width="35"/>
-    <col customWidth="1" max="7" min="7" style="3" width="32.1666666666667"/>
+    <col customWidth="1" max="7" min="7" style="3" width="32.1640625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="28.8" r="1" s="3" spans="1:8">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +838,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
 </worksheet>
@@ -1474,7 +856,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
 </worksheet>

</xml_diff>